<commit_message>
changes to the story while recording
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Story/Resources/Story.xlsx
+++ b/Assets/Scripts/Story/Resources/Story.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\My Important Files\My TUDelft\Informatica\Msc 1\The Legend of Iris\Assets\Scripts\Story\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivier\Documents\TUDelft\Building Serious Games\Legend-Of-Iris\Assets\Scripts\Story\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="360">
   <si>
     <t>T0.1</t>
   </si>
@@ -42,9 +42,6 @@
     <t>*tuuuut*tuuuut* You have 1 incoming call from *“Lucy”*. Connecting you through now.</t>
   </si>
   <si>
-    <t>*phone effect* Hello? Human? I need your help!! Are you there? Please press up/down/left/right in that order, to confirm you can hear me and that the connection is properly working.</t>
-  </si>
-  <si>
     <t>T1.2</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>Ha.ha.ha.</t>
   </si>
   <si>
-    <t>Just press forward to confirm. Will you help us, human?</t>
-  </si>
-  <si>
     <t>T1.4</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>Forward and backward movement enabled.</t>
   </si>
   <si>
-    <t xml:space="preserve">Let’s see if you can move him. Press forward and backward to move Beorn. </t>
-  </si>
-  <si>
     <t>T2.2</t>
   </si>
   <si>
@@ -153,9 +144,6 @@
     <t>Rotations enabled.</t>
   </si>
   <si>
-    <t>Let’s try and see if you can turn Beorn around in order to look at a different direction. First do a full rotation to the left.</t>
-  </si>
-  <si>
     <t>Press the left or right keys to turn left or right.</t>
   </si>
   <si>
@@ -222,15 +210,9 @@
     <t>*happy* muumumuuuu!!</t>
   </si>
   <si>
-    <t xml:space="preserve">Well done, human!! Notice how the sound changes when you turn? You should pay close attention attention to the changes of audio in order to orient yourself. </t>
-  </si>
-  <si>
     <t>T3.1</t>
   </si>
   <si>
-    <t>Alright, you are ready to try walking around! Before we can get to the spirit village, we should get Beorn ready to move out. First he needs his shoes, and second… well… he needs to unplug his belly rubbing machine. He doesn’t like it when devices are on stand-by when he leaves the house. It may start a fire, you know? Let’s first move Beorn to his shoes. I’ll fly over to their location, so you may follow the sound of my wings.</t>
-  </si>
-  <si>
     <t>T3.2</t>
   </si>
   <si>
@@ -279,9 +261,6 @@
     <t xml:space="preserve">Good, Beorn! You can get a belly rub later, when you come back home.. </t>
   </si>
   <si>
-    <t xml:space="preserve">Alright, human! Let’s head to the door so we can get out of this place. It smell funky in here. You should be glad you are not connected to Beorn by smell! It smells like my grandma’s feet, when she doesn’t shower for a month. </t>
-  </si>
-  <si>
     <t>Quickly, follow me!</t>
   </si>
   <si>
@@ -342,9 +321,6 @@
     <t>Haha!</t>
   </si>
   <si>
-    <t xml:space="preserve">By the way, human, as you noticed I have magical powers! If something significant happens, I get my spirit juices flowing through my magnificent body! The spirit world then opens up highly concentrated Wibbly Wobbly Timey Wimey spirit magic locations where I can teleport Beorn to. Whenever he falls off, I will teleport him back to the beginning of the bridge section he fell off from. </t>
-  </si>
-  <si>
     <t>Alright! Let’s cross this bridge! Follow me!</t>
   </si>
   <si>
@@ -423,9 +399,6 @@
     <t>*glad* muu!</t>
   </si>
   <si>
-    <t>Well done! Now the next segment. Follow me!</t>
-  </si>
-  <si>
     <t>T4.5*2</t>
   </si>
   <si>
@@ -477,9 +450,6 @@
     <t>*happy* mu muuu</t>
   </si>
   <si>
-    <t>Awesome!! Well done. Okay, let’s continue over the next section.</t>
-  </si>
-  <si>
     <t>T4.9*2</t>
   </si>
   <si>
@@ -528,9 +498,6 @@
     <t>*very happy* muu muu muuuuuu!</t>
   </si>
   <si>
-    <t>Very goood!! We reached the end of the bridge. Here is a portal to my village. Beorn, don’t be scared, you might feel some dizziness and lightheadedness, but that is normal. Here we go!! woooop!</t>
-  </si>
-  <si>
     <t>*awesome teleportation sounds*</t>
   </si>
   <si>
@@ -984,9 +951,6 @@
     <t>Lucy! *hoot* Teleport us into a big empty hall!!</t>
   </si>
   <si>
-    <t>I have never heard anyone be so happy to go to a big hall to test echoing farts. Here we go *teleport sounds*</t>
-  </si>
-  <si>
     <t>Awesome!! Ok, *Beorns of stomach* here goes nothing....  *difficult hoot* *pfffff*...fff*..ff*..f*</t>
   </si>
   <si>
@@ -1075,13 +1039,73 @@
   </si>
   <si>
     <t>lucy</t>
+  </si>
+  <si>
+    <t>*phone effect* Hello? Human? I need your help!! Are you there? Please press up/down/left/right in that order to confirm you can hear me and that the connection is properly working.</t>
+  </si>
+  <si>
+    <t>Don’t listen to iris! Just press forward to confirm. Will you help us, human?</t>
+  </si>
+  <si>
+    <t>ber cald beeoorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Now, let’s see if you can move him. Press forward and backward to move Beorn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haha, aww poor Beorn. He fell down, but that's okay. He is quite strong and has a lot of fur to break his fall. He is a bit clumsy sometimes though. At least he is fully awake now! </t>
+  </si>
+  <si>
+    <t>Let’s try and see if you can turn Beorn around. First, do a full rotation to the left.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Well done, human!! Notice how the sound changes when you turn? You should pay close attention to the changes of audio in order to orient yourself. </t>
+  </si>
+  <si>
+    <t>Alright, you are ready to try walking around! Before we can get to the spirit village, we should get Beorn ready to move out. First he needs his shoes, and second… well… he needs to unplug his belly rubbing machine. He doesn’t like it when devices are on stand-by when he leaves the house. It may start a fire, you know?       Let’s first walk Beorn to his shoes. I’ll fly over to their location, so you may follow the sound of my wings.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahh!! Science!! </t>
+  </si>
+  <si>
+    <t>noooo not science!</t>
+  </si>
+  <si>
+    <t>blegh science birds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thanks, human, for clearing the forest. Now that the science birds have stopped their experiments, I can now finally go back in peace. Hoorayyy! </t>
+  </si>
+  <si>
+    <t>Mom!! I'm coming back home!! From now on I will eat all your vegetables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alright, human! Let’s head to the door so we can get out of this place. It smells funky in here. You should be glad you are not connected to Beorn by smell! It smells like my grandma’s feet, when she doesn’t shower for a month. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">By the way, human, as you noticed I have magical powers! If something significant happens, I get my spirit juices flowing through my magnificent body! The spirit world then opens up spirit locations with highly concentrated Wibbly Wobbly Timey Wimey spirit magic stuff where I can  teleport Beorn to. Whenever he falls off, I will teleport him back to the beginning of the bridge section he fell off from. </t>
+  </si>
+  <si>
+    <t>Well done! Now the next section. Follow me!</t>
+  </si>
+  <si>
+    <t>Awesome!! Well done. Okay, let’s continue over to the next section.</t>
+  </si>
+  <si>
+    <t>Very goood!! We have reached the end of the bridge. Here we will now take the portal to my village. Beorn, don’t be scared, you might feel a bit dizzy, but that is normal. Here we go!! woooop!</t>
+  </si>
+  <si>
+    <t>seventie seventh</t>
+  </si>
+  <si>
+    <t>Okidoki!! Here we go *teleport sounds*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1216,8 +1240,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1403,6 +1433,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1564,12 +1600,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1891,18 +1929,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C325"/>
+  <dimension ref="A1:D333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A310" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C315" sqref="C315"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="57.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1944,42 +1983,42 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1987,15 +2026,15 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2003,15 +2042,15 @@
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2019,169 +2058,172 @@
         <v>1</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B18" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>21</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>29</v>
       </c>
       <c r="B25" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C30" s="2" t="s">
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>42</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2189,39 +2231,39 @@
         <v>1</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>44</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C37" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -2229,39 +2271,39 @@
         <v>1</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>44</v>
+        <v>345</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C42" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -2269,2282 +2311,2285 @@
         <v>1</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C47" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C59" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>69</v>
+        <v>347</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C80" s="2" t="s">
-        <v>86</v>
+        <v>353</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C82" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="C102" s="2" t="s">
-        <v>107</v>
+        <v>354</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C104" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B113" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B117" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B119" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>134</v>
+        <v>355</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B130" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B140" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B145" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B147" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B148" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>152</v>
+        <v>356</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B149" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B152" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B156" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B158" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>157</v>
+      </c>
+      <c r="B160" t="s">
+        <v>30</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B161" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>73</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>160</v>
+      </c>
+      <c r="B163" t="s">
+        <v>73</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B164" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>30</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B166" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B167" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B168" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C168" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B160" t="s">
-        <v>32</v>
-      </c>
-      <c r="C160" s="2" t="s">
+    </row>
+    <row r="169" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B169" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C169" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B161" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C161" s="2" t="s">
+    <row r="170" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B170" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C170" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
-        <v>79</v>
-      </c>
-      <c r="C162" s="2" t="s">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B171" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C171" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>73</v>
+      </c>
+      <c r="C172" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B163" t="s">
-        <v>79</v>
-      </c>
-      <c r="C163" s="2" t="s">
+    </row>
+    <row r="173" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B173" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C173" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B164" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>32</v>
-      </c>
-      <c r="C165" s="2" t="s">
+      <c r="D173" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>173</v>
+      </c>
+      <c r="C174" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B166" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C166" s="2" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C175" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B167" t="s">
+    <row r="176" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>173</v>
+      </c>
+      <c r="C176" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B168" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="B169" t="s">
-        <v>176</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B170" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B171" t="s">
-        <v>176</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
-        <v>79</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B173" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>184</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B175" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>184</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B177" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B180" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="B181" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="B182" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="B183" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="B184" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B185" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B187" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B189" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="B195" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B205" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="B206" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B210" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B211" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B213" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B215" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B216" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B217" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B220" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B222" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B224" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B225" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B226" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B227" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B230" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="B231" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B233" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B234" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B235" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B237" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="B239" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B241" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="B242" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B243" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="B245" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B246" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="B247" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B249" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C250" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B255" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="B263" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B264" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B266" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B267" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B269" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B270" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="B275" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="276" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B278" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B280" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="282" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B282" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B289" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="B291" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B294" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="C294" s="2" t="s">
-        <v>321</v>
+        <v>339</v>
+      </c>
+      <c r="C294" s="4" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B296" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B298" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="299" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="B299" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C306" s="2" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="C308" s="2" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C310" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C312" s="2" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B313" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B315" s="1" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -4552,48 +4597,73 @@
         <v>1</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="B318" t="s">
         <v>1</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C319" s="2" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C320" s="2" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="321" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C321" s="2" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="322" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C322" s="2" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
     </row>
     <row r="323" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C323" s="2" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="325" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C325" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C329" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C330" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C331" s="2" t="s">
         <v>350</v>
+      </c>
+    </row>
+    <row r="332" spans="3:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C332" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C333" s="2" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further changes to the story script, while I am recording the voices
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Story/Resources/Story.xlsx
+++ b/Assets/Scripts/Story/Resources/Story.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="360">
   <si>
     <t>T0.1</t>
   </si>
@@ -834,9 +834,6 @@
     <t>Oh oh *hoot*, I can see spirit crows approaching</t>
   </si>
   <si>
-    <t>*whistle* Oh did I forget to mention, that crows also respond our emergency calls? It is a problem we still haven’t figured out how to avoid.</t>
-  </si>
-  <si>
     <t>Ok, human, birds will be flying passed you. Only grab the science birds *hoot*, so listen carefully to their calls. Whenever you do catch a crow, you have to bring it to Lucy. She will then keep it in a cage for now. Good luck! *hoot*</t>
   </si>
   <si>
@@ -897,9 +894,6 @@
     <t xml:space="preserve">Yes! You have one! *hoot* Let's test it. Bird, if I make noise a kilometer away from you, how long does it take for you to hear it? </t>
   </si>
   <si>
-    <t>Well, 1 kilometer is a 1000 meters and sound travels roughly 335 meters per second through air. 1000 divided by 335 is about 3. Therefore, 3 seconds after the mentioned disgusting event, you will hear it.</t>
-  </si>
-  <si>
     <t>Let's test this!! Luckily, I have a friend who is currently 1 kilometer away from us. Let’s call him and ask if he can make some noise. *dial tones, ringing* yooo bro! I am conducting an experiment and I need you to do the thing!</t>
   </si>
   <si>
@@ -921,9 +915,6 @@
     <t>YAY! Another one! Let's test him too.  Bird, when something passes by quickly, why does the tone change?</t>
   </si>
   <si>
-    <t>That is called the Doppler effect. Whenever an object comes towards you, the sound waves coming from that object, are more compressed! Therefore, the sound sounds higher pitched. If the object would move away from you, the sound waves are stretched so it sounds... can you guess it?.... yes! lower!!</t>
-  </si>
-  <si>
     <t>Okay.. Let me fly by you a few times. Tell me if he is right.</t>
   </si>
   <si>
@@ -945,9 +936,6 @@
     <t>Aha! The final one. Let's test it to be sure. Bird, if I make noise in a big empty hall, why do I hear it repeated?</t>
   </si>
   <si>
-    <t>Easy! That is called an echo! Sound waves are partially absorbed by objects in your environment, and partially bounced back. So some sound waves might have bounced on other objects before reaching your ears, while some other waves reach you directly. Since it takes time for sound to travel from the source to your ear, it takes even longer for bounced sound waves to reach your ears, so that you hear the sound a bit later too.</t>
-  </si>
-  <si>
     <t>Lucy! *hoot* Teleport us into a big empty hall!!</t>
   </si>
   <si>
@@ -984,12 +972,6 @@
     <t>Haha ah! *whistle* Thank you, Boris!</t>
   </si>
   <si>
-    <t>Human, you seem very talented! I see you are motivated to learn how to orient even better by the use of sound. So, let me tell you a secret. *whistle*</t>
-  </si>
-  <si>
-    <t>If you listen well and practise enough, you could roughly determine the dimensions and type of environment you are in, just by the use of sound. You could possibly even learn to hear if there is a wall in front of you. The key here, is the effect that sound has in an environment. Sound waves travel and bounce around, and since each environment is different, the bounced sound waves are also different. Let’s call this the response of an environment. *whistle*</t>
-  </si>
-  <si>
     <t>Some hearing impaired humans can distinguish these responses, just by making clicking sounds. They listen to the response in the environment just like bats do. *whistle*</t>
   </si>
   <si>
@@ -1099,6 +1081,24 @@
   </si>
   <si>
     <t>Okidoki!! Here we go *teleport sounds*</t>
+  </si>
+  <si>
+    <t>*whistle* Oh did I forget to mention, that crows also respond our emergency calls? Yeahhh, it is a problem we still haven't figured out.</t>
+  </si>
+  <si>
+    <t>Well, 1 kilometer is a 1000 meters and sound travels roughly 335 meters per second through air. 1000 divided by 335 is about 3. Therefore, if you were to make a loud noise 1 kilometer away, we would hear it 3 seconds later.</t>
+  </si>
+  <si>
+    <t>That is called the Doppler effect. Whenever an object comes towards you, the sound waves coming from that object, are more compressed! Therefore, the sound sounds higher pitched. If the object moves away from you, the sound waves are stretched so it sounds... can you guess it?.... yes! lower!!</t>
+  </si>
+  <si>
+    <t>Easy! That is called an echo! Sound waves are partially absorbed and partially reflected by objects in your environment, such as a cup, a wall, or a MOUNTAIN. So before reaching your ears, some sound waves have bounced on other objects, while other waves reach your ears directly. Since it takes time for sound to travel from the source to your ear, it takes even longer for reflected sound waves, so you hear that sound a bit later.</t>
+  </si>
+  <si>
+    <t>Human, you seem very talented! I see you are motivated to learn how to orientate yourself even better by the use of sound. So, let me tell you a secret. *whistle*</t>
+  </si>
+  <si>
+    <t>If you listen well and practise enough, you can roughly determine the dimensions and type of environment you are in, just by the sound. You could even learn to hear if there is a wall in front of you. The key here, is the effect that sound has in an environment. Sound waves travel and bounce around, and since each environment is different, the bounced sound waves are also different. Let’s call this the response of an environment. Even your position in relation to your surroundings influences the response. *whistle*</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1247,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1439,6 +1439,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1600,7 +1606,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1608,6 +1614,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1931,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A310" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C315" sqref="C315"/>
+    <sheetView tabSelected="1" topLeftCell="B309" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D317" sqref="D317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1985,10 +1992,10 @@
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1996,7 +2003,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>8</v>
@@ -2015,7 +2022,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
@@ -2031,7 +2038,7 @@
     </row>
     <row r="13" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
@@ -2047,7 +2054,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
@@ -2063,10 +2070,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2074,7 +2081,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
@@ -2085,7 +2092,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>20</v>
@@ -2104,7 +2111,7 @@
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>23</v>
@@ -2128,7 +2135,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>26</v>
@@ -2147,13 +2154,13 @@
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2166,7 +2173,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>32</v>
@@ -2182,10 +2189,10 @@
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2201,7 +2208,7 @@
     </row>
     <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>36</v>
@@ -2220,10 +2227,10 @@
     </row>
     <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2236,10 +2243,10 @@
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -2260,7 +2267,7 @@
     </row>
     <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>39</v>
@@ -2276,10 +2283,10 @@
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2300,7 +2307,7 @@
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>39</v>
@@ -2316,10 +2323,10 @@
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -2340,7 +2347,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>47</v>
@@ -2359,7 +2366,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>49</v>
@@ -2378,7 +2385,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>51</v>
@@ -2397,7 +2404,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>54</v>
@@ -2421,7 +2428,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>54</v>
@@ -2445,7 +2452,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>60</v>
@@ -2464,10 +2471,10 @@
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -2475,10 +2482,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2494,7 +2501,7 @@
     </row>
     <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>65</v>
@@ -2513,7 +2520,7 @@
     </row>
     <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>68</v>
@@ -2529,7 +2536,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>70</v>
@@ -2548,7 +2555,7 @@
     </row>
     <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>65</v>
@@ -2575,7 +2582,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>76</v>
@@ -2599,7 +2606,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>79</v>
@@ -2607,7 +2614,7 @@
     </row>
     <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C80" s="2" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2628,7 +2635,7 @@
     </row>
     <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>65</v>
@@ -2647,7 +2654,7 @@
     </row>
     <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>84</v>
@@ -2666,7 +2673,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>87</v>
@@ -2682,7 +2689,7 @@
     </row>
     <row r="90" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>89</v>
@@ -2698,7 +2705,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>91</v>
@@ -2730,7 +2737,7 @@
     </row>
     <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>95</v>
@@ -2746,7 +2753,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>97</v>
@@ -2762,7 +2769,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>99</v>
@@ -2770,7 +2777,7 @@
     </row>
     <row r="102" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="C102" s="2" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -2791,7 +2798,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>103</v>
@@ -2807,7 +2814,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>104</v>
@@ -2826,7 +2833,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>106</v>
@@ -2842,7 +2849,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>107</v>
@@ -2861,7 +2868,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>110</v>
@@ -2877,7 +2884,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C116" s="2" t="s">
         <v>111</v>
@@ -2896,7 +2903,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>114</v>
@@ -2915,7 +2922,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>117</v>
@@ -2934,7 +2941,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>120</v>
@@ -2953,7 +2960,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>123</v>
@@ -2972,10 +2979,10 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -2991,7 +2998,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>128</v>
@@ -3002,7 +3009,7 @@
         <v>129</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>130</v>
@@ -3029,7 +3036,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>103</v>
@@ -3045,7 +3052,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>104</v>
@@ -3072,7 +3079,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>106</v>
@@ -3088,7 +3095,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>107</v>
@@ -3115,7 +3122,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>110</v>
@@ -3131,7 +3138,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>111</v>
@@ -3150,7 +3157,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>140</v>
@@ -3169,10 +3176,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B148" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3188,7 +3195,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>145</v>
@@ -3199,7 +3206,7 @@
         <v>146</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>147</v>
@@ -3218,7 +3225,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B153" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>149</v>
@@ -3234,7 +3241,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>150</v>
@@ -3253,7 +3260,7 @@
     </row>
     <row r="157" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>153</v>
@@ -3272,7 +3279,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>156</v>
@@ -3291,10 +3298,10 @@
     </row>
     <row r="161" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B161" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -3318,7 +3325,7 @@
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>162</v>
@@ -3334,7 +3341,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>164</v>
@@ -3350,7 +3357,7 @@
     </row>
     <row r="168" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>167</v>
@@ -3366,7 +3373,7 @@
     </row>
     <row r="170" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>169</v>
@@ -3390,13 +3397,13 @@
     </row>
     <row r="173" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>172</v>
       </c>
       <c r="D173" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3409,7 +3416,7 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B175" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>175</v>
@@ -3425,7 +3432,7 @@
     </row>
     <row r="177" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B177" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>177</v>
@@ -3449,7 +3456,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B180" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>180</v>
@@ -3501,7 +3508,7 @@
     </row>
     <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B185" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>187</v>
@@ -3536,7 +3543,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B189" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>191</v>
@@ -3576,7 +3583,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>194</v>
@@ -3611,7 +3618,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>197</v>
@@ -3638,7 +3645,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>201</v>
@@ -3670,7 +3677,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B205" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>205</v>
@@ -3697,7 +3704,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>209</v>
@@ -3713,7 +3720,7 @@
     </row>
     <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B210" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>211</v>
@@ -3740,7 +3747,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B213" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>106</v>
@@ -3756,7 +3763,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B215" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>215</v>
@@ -3775,7 +3782,7 @@
     </row>
     <row r="217" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B217" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C217" s="2" t="s">
         <v>218</v>
@@ -3786,7 +3793,7 @@
         <v>219</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>220</v>
@@ -3802,7 +3809,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B220" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>222</v>
@@ -3848,7 +3855,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B225" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>114</v>
@@ -3867,7 +3874,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B227" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C227" s="2" t="s">
         <v>230</v>
@@ -3891,7 +3898,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B230" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>233</v>
@@ -3918,7 +3925,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B233" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>233</v>
@@ -3937,7 +3944,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B235" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>238</v>
@@ -3953,7 +3960,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B237" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>240</v>
@@ -3988,7 +3995,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B241" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>245</v>
@@ -4007,7 +4014,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B243" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>248</v>
@@ -4034,7 +4041,7 @@
     </row>
     <row r="246" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B246" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>250</v>
@@ -4076,7 +4083,7 @@
       </c>
     </row>
     <row r="251" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B251" t="s">
+      <c r="B251" s="5" t="s">
         <v>256</v>
       </c>
       <c r="C251" s="2" t="s">
@@ -4092,7 +4099,7 @@
       </c>
     </row>
     <row r="253" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B253" t="s">
+      <c r="B253" s="5" t="s">
         <v>256</v>
       </c>
       <c r="C253" s="2" t="s">
@@ -4111,7 +4118,7 @@
       <c r="A255" t="s">
         <v>261</v>
       </c>
-      <c r="B255" t="s">
+      <c r="B255" s="5" t="s">
         <v>256</v>
       </c>
       <c r="C255" s="2" t="s">
@@ -4119,7 +4126,7 @@
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B256" t="s">
+      <c r="B256" s="5" t="s">
         <v>263</v>
       </c>
       <c r="C256" s="2" t="s">
@@ -4127,7 +4134,7 @@
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B257" t="s">
+      <c r="B257" s="5" t="s">
         <v>265</v>
       </c>
       <c r="C257" s="2" t="s">
@@ -4135,7 +4142,7 @@
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B258" t="s">
+      <c r="B258" s="5" t="s">
         <v>267</v>
       </c>
       <c r="C258" s="2" t="s">
@@ -4143,7 +4150,7 @@
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B259" t="s">
+      <c r="B259" s="5" t="s">
         <v>256</v>
       </c>
       <c r="C259" s="2" t="s">
@@ -4159,11 +4166,11 @@
       </c>
     </row>
     <row r="261" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B261" t="s">
+      <c r="B261" s="5" t="s">
         <v>256</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>271</v>
+        <v>354</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4171,140 +4178,140 @@
         <v>173</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
+        <v>272</v>
+      </c>
+      <c r="B263" t="s">
+        <v>30</v>
+      </c>
+      <c r="C263" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="B263" t="s">
-        <v>30</v>
-      </c>
-      <c r="C263" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B264" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
+        <v>275</v>
+      </c>
+      <c r="C265" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C265" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
+        <v>277</v>
+      </c>
+      <c r="B266" t="s">
+        <v>30</v>
+      </c>
+      <c r="C266" s="2" t="s">
         <v>278</v>
-      </c>
-      <c r="B266" t="s">
-        <v>30</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B267" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
+        <v>275</v>
+      </c>
+      <c r="C268" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
+        <v>280</v>
+      </c>
+      <c r="B269" t="s">
+        <v>30</v>
+      </c>
+      <c r="C269" s="2" t="s">
         <v>281</v>
-      </c>
-      <c r="B269" t="s">
-        <v>30</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B270" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
+        <v>275</v>
+      </c>
+      <c r="C271" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C271" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
+        <v>283</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C272" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="B272" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C272" s="2" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>285</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C273" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="B273" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C273" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
+        <v>287</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C274" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="B274" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C274" s="2" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="275" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
+        <v>289</v>
+      </c>
+      <c r="B275" t="s">
+        <v>173</v>
+      </c>
+      <c r="C275" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="B275" t="s">
-        <v>173</v>
-      </c>
-      <c r="C275" s="2" t="s">
-        <v>291</v>
-      </c>
     </row>
     <row r="276" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B276" t="s">
+      <c r="B276" s="5" t="s">
         <v>263</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>292</v>
+        <v>355</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -4312,15 +4319,15 @@
         <v>173</v>
       </c>
       <c r="C277" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B278" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -4328,15 +4335,15 @@
         <v>73</v>
       </c>
       <c r="C279" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B280" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C280" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="281" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4344,26 +4351,26 @@
         <v>173</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="282" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B282" t="s">
         <v>173</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B283" t="s">
+      <c r="B283" s="5" t="s">
         <v>265</v>
       </c>
       <c r="C283" s="2" t="s">
-        <v>300</v>
+        <v>356</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -4371,7 +4378,7 @@
         <v>173</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -4379,7 +4386,7 @@
         <v>173</v>
       </c>
       <c r="C285" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -4387,7 +4394,7 @@
         <v>173</v>
       </c>
       <c r="C286" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -4395,7 +4402,7 @@
         <v>173</v>
       </c>
       <c r="C287" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
@@ -4403,15 +4410,15 @@
         <v>173</v>
       </c>
       <c r="C288" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B289" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C289" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
@@ -4419,26 +4426,26 @@
         <v>173</v>
       </c>
       <c r="C290" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B291" t="s">
         <v>173</v>
       </c>
       <c r="C291" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B292" t="s">
+      <c r="B292" s="5" t="s">
         <v>267</v>
       </c>
       <c r="C292" s="2" t="s">
-        <v>308</v>
+        <v>357</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
@@ -4446,15 +4453,15 @@
         <v>173</v>
       </c>
       <c r="C293" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="294" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
       <c r="B294" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C294" s="4" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4462,15 +4469,15 @@
         <v>173</v>
       </c>
       <c r="C295" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B296" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C296" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -4478,34 +4485,34 @@
         <v>173</v>
       </c>
       <c r="C297" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B298" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C298" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B299" t="s">
         <v>173</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B300" t="s">
+      <c r="B300" s="5" t="s">
         <v>265</v>
       </c>
       <c r="C300" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
@@ -4513,15 +4520,15 @@
         <v>173</v>
       </c>
       <c r="C301" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B302" t="s">
+      <c r="B302" s="5" t="s">
         <v>265</v>
       </c>
       <c r="C302" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -4529,43 +4536,49 @@
         <v>173</v>
       </c>
       <c r="C303" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B304" t="s">
+      <c r="B304" s="5" t="s">
         <v>265</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="306" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C306" s="2" t="s">
-        <v>321</v>
+        <v>358</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B308" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="C308" s="2" t="s">
-        <v>322</v>
+        <v>359</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B310" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="C310" s="2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C312" s="2" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B313" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C313" s="2" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -4573,23 +4586,23 @@
         <v>173</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B315" s="1" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -4597,73 +4610,73 @@
         <v>1</v>
       </c>
       <c r="C317" s="2" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B318" t="s">
         <v>1</v>
       </c>
       <c r="C318" s="2" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C319" s="2" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C320" s="2" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="321" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C321" s="2" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="322" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C322" s="2" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="323" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C323" s="2" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="325" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C325" s="2" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="329" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C329" s="2" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="330" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C330" s="2" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="331" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C331" s="2" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="332" spans="3:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C332" s="2" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="333" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C333" s="2" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes while recording, and settings text updated in docx
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Story/Resources/Story.xlsx
+++ b/Assets/Scripts/Story/Resources/Story.xlsx
@@ -600,9 +600,6 @@
     <t>*disappointed* muhhhh</t>
   </si>
   <si>
-    <t>*hOOOt* Oh fudge, now my feathers are all messy. Ah, well.  I needed a haircut anyway. Right, where was I. *hooot* Oh yes: let's try again and see if you got lucky!!</t>
-  </si>
-  <si>
     <t>OK, let’s go find him again!</t>
   </si>
   <si>
@@ -690,9 +687,6 @@
     <t>Let's continue quickly</t>
   </si>
   <si>
-    <t>Perhaps I will install a frog shower at the swamp one day. *hooot* For now, let’s move on! We'll move to the clearing where I heard the birds are located. Follow me and Lucy, Human! *hooot*</t>
-  </si>
-  <si>
     <t>T6.5</t>
   </si>
   <si>
@@ -714,9 +708,6 @@
     <t>Beorn! Leave those poor flies alone!</t>
   </si>
   <si>
-    <t>Human, What is the difference between a fly and a bird? A bird can fly but a fly can't bird! *hoot* HUAHUAHUAH</t>
-  </si>
-  <si>
     <t>huehuehue</t>
   </si>
   <si>
@@ -750,9 +741,6 @@
     <t>T6.10</t>
   </si>
   <si>
-    <t>Ahhh! yes! here we are. The science bird must be around here!</t>
-  </si>
-  <si>
     <t>*glad* muuuu!</t>
   </si>
   <si>
@@ -915,9 +903,6 @@
     <t>YAY! Another one! Let's test him too.  Bird, when something passes by quickly, why does the tone change?</t>
   </si>
   <si>
-    <t>Okay.. Let me fly by you a few times. Tell me if he is right.</t>
-  </si>
-  <si>
     <t>wiiiiiiiiiiiiiiiiiiii</t>
   </si>
   <si>
@@ -939,9 +924,6 @@
     <t>Lucy! *hoot* Teleport us into a big empty hall!!</t>
   </si>
   <si>
-    <t>Awesome!! Ok, *Beorns of stomach* here goes nothing....  *difficult hoot* *pfffff*...fff*..ff*..f*</t>
-  </si>
-  <si>
     <t>OK! ENOUGH! Ugh, who gives our king beans for dinner??</t>
   </si>
   <si>
@@ -954,9 +936,6 @@
     <t>T9.1</t>
   </si>
   <si>
-    <t>Ahhh *hoooot* home sweet home. Thank you human, for your exceptional help. You are very talented, and will achieve a great many things!! I'll soon bring back these science birds back to science land.</t>
-  </si>
-  <si>
     <t>NO!! *whistle* Wait! You can take my friends, but let me stay here!! Our study hasn’t been completed, I’d like to finish it. Plus, I like it here. It smells so good, and the air feels so nice and soft. Everyone here seems so friendly too.</t>
   </si>
   <si>
@@ -1099,13 +1078,34 @@
   </si>
   <si>
     <t>If you listen well and practise enough, you can roughly determine the dimensions and type of environment you are in, just by the sound. You could even learn to hear if there is a wall in front of you. The key here, is the effect that sound has in an environment. Sound waves travel and bounce around, and since each environment is different, the bounced sound waves are also different. Let’s call this the response of an environment. Even your position in relation to your surroundings influences the response. *whistle*</t>
+  </si>
+  <si>
+    <t>*hOOOt* Oh fudge, now my feathers are all messy. Ah, well.  I needed a feathercut anyway. Right, where was I. *hooot* Oh yes: let's try again and see if you got lucky!!</t>
+  </si>
+  <si>
+    <t>Perhaps I will install a frog shower at the swamp one day. *hooot* For now, let’s move on! We'll move to the clearing where the birds are supposed to be. Follow me and Lucy, Human! *hooot*</t>
+  </si>
+  <si>
+    <t>Human, what is the difference between a fly and a bird? A bird can fly but a fly can't bird! *hoot* HUAHUAHUAH</t>
+  </si>
+  <si>
+    <t>Ahhh! yes! here we are. The science bird must be around here somewhere!</t>
+  </si>
+  <si>
+    <t>Okay.. Let me fly by you a few times. Tell me if he's right.</t>
+  </si>
+  <si>
+    <t>Awesome!! Ok, *grumbles of stomach* here goes nothing....  *difficult hoot* *pfffff*...fff*..ff*..f*</t>
+  </si>
+  <si>
+    <t>Ahhh *hoooot* home sweet home. Thank you human, for your exceptional help. You are very talented, and will achieve many great things!! I'll soon bring these science birds back to science land.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1241,13 +1241,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Trebuchet MS"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1429,19 +1441,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1606,15 +1606,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1938,13 +1939,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B309" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D317" sqref="D317"/>
+    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="C314" sqref="C314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="72.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="72.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1952,30 +1954,30 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1983,29 +1985,29 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>334</v>
+      <c r="B8" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2013,77 +2015,77 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>335</v>
+      <c r="B17" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2091,10 +2093,10 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2102,42 +2104,42 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="B21" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2145,72 +2147,72 @@
       <c r="A25" t="s">
         <v>27</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="B26" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D26" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="B28" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>337</v>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="B31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C32" s="2" t="s">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2218,39 +2220,39 @@
       <c r="A33" t="s">
         <v>37</v>
       </c>
-      <c r="B33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>338</v>
+      <c r="B34" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>339</v>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2258,39 +2260,39 @@
       <c r="A38" t="s">
         <v>42</v>
       </c>
-      <c r="B38" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="2" t="s">
+      <c r="B38" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="B39" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>339</v>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="1" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2298,39 +2300,39 @@
       <c r="A43" t="s">
         <v>44</v>
       </c>
-      <c r="B43" t="s">
-        <v>30</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="B43" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C44" s="2" t="s">
+      <c r="B44" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>339</v>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2338,18 +2340,18 @@
       <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
-        <v>30</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="B48" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="B49" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2357,18 +2359,18 @@
       <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="B50" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B51" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2376,18 +2378,18 @@
       <c r="A52" t="s">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
-        <v>30</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="B52" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="B53" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2395,23 +2397,23 @@
       <c r="A54" t="s">
         <v>52</v>
       </c>
-      <c r="B54" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54" s="2" t="s">
+      <c r="B54" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C55" s="2" t="s">
+      <c r="B55" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
@@ -2419,23 +2421,23 @@
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B57" t="s">
-        <v>30</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="B57" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="B58" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="1" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2443,18 +2445,18 @@
       <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
-        <v>30</v>
-      </c>
-      <c r="C60" s="2" t="s">
+      <c r="B60" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="B61" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2462,48 +2464,48 @@
       <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" t="s">
-        <v>30</v>
-      </c>
-      <c r="C62" s="2" t="s">
+      <c r="B62" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>333</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>341</v>
+      <c r="B64" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
-        <v>30</v>
-      </c>
-      <c r="C65" s="2" t="s">
+      <c r="B65" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B66" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C66" s="2" t="s">
+      <c r="B66" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2511,34 +2513,34 @@
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
-        <v>30</v>
-      </c>
-      <c r="C67" s="2" t="s">
+      <c r="B67" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C68" s="2" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>30</v>
-      </c>
-      <c r="C69" s="2" t="s">
+      <c r="B69" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="B70" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2546,18 +2548,18 @@
       <c r="A71" t="s">
         <v>71</v>
       </c>
-      <c r="B71" t="s">
-        <v>30</v>
-      </c>
-      <c r="C71" s="2" t="s">
+      <c r="B71" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C72" s="2" t="s">
+      <c r="B72" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2565,60 +2567,60 @@
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C73" s="2" t="s">
+      <c r="C73" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>30</v>
-      </c>
-      <c r="C74" s="2" t="s">
+      <c r="B74" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C75" s="2" t="s">
+      <c r="B75" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="B76" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" s="2" t="s">
+      <c r="B77" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C78" s="2" t="s">
+      <c r="B78" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="C80" s="2" t="s">
-        <v>347</v>
+      <c r="C80" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2626,18 +2628,18 @@
       <c r="A83" t="s">
         <v>81</v>
       </c>
-      <c r="B83" t="s">
-        <v>30</v>
-      </c>
-      <c r="C83" s="2" t="s">
+      <c r="B83" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C84" s="2" t="s">
+      <c r="B84" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2645,26 +2647,26 @@
       <c r="A85" t="s">
         <v>82</v>
       </c>
-      <c r="B85" t="s">
-        <v>30</v>
-      </c>
-      <c r="C85" s="2" t="s">
+      <c r="B85" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B86" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C86" s="2" t="s">
+      <c r="B86" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+      <c r="B87" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2672,116 +2674,116 @@
       <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C88" s="2" t="s">
+      <c r="B88" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
-        <v>30</v>
-      </c>
-      <c r="C89" s="2" t="s">
+      <c r="B89" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B90" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C90" s="2" t="s">
+      <c r="B90" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>30</v>
-      </c>
-      <c r="C91" s="2" t="s">
+      <c r="B91" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C92" s="2" t="s">
+      <c r="B92" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>30</v>
-      </c>
-      <c r="C93" s="2" t="s">
+      <c r="B93" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B94" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
-        <v>30</v>
-      </c>
-      <c r="C95" s="2" t="s">
+      <c r="B95" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B96" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C96" s="2" t="s">
+      <c r="B96" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B97" t="s">
-        <v>30</v>
-      </c>
-      <c r="C97" s="2" t="s">
+      <c r="B97" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C98" s="2" t="s">
+      <c r="B98" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B99" t="s">
-        <v>30</v>
-      </c>
-      <c r="C99" s="2" t="s">
+      <c r="B99" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C100" s="2" t="s">
+      <c r="B100" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="C102" s="2" t="s">
-        <v>348</v>
+    <row r="102" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="C102" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C104" s="2" t="s">
+      <c r="C104" s="1" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2789,34 +2791,34 @@
       <c r="A105" t="s">
         <v>101</v>
       </c>
-      <c r="B105" t="s">
-        <v>30</v>
-      </c>
-      <c r="C105" s="2" t="s">
+      <c r="B105" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C106" s="2" t="s">
+      <c r="B106" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C106" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
+      <c r="B107" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C108" s="2" t="s">
+      <c r="B108" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C108" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2824,34 +2826,34 @@
       <c r="A109" t="s">
         <v>105</v>
       </c>
-      <c r="B109" t="s">
-        <v>30</v>
-      </c>
-      <c r="C109" s="2" t="s">
+      <c r="B109" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C109" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C110" s="2" t="s">
+      <c r="B110" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C110" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
+      <c r="B111" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C112" s="2" t="s">
+      <c r="B112" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2859,34 +2861,34 @@
       <c r="A113" t="s">
         <v>108</v>
       </c>
-      <c r="B113" t="s">
-        <v>30</v>
-      </c>
-      <c r="C113" s="2" t="s">
+      <c r="B113" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B114" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C114" s="2" t="s">
+      <c r="B114" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
+      <c r="B115" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B116" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C116" s="2" t="s">
+      <c r="B116" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2894,18 +2896,18 @@
       <c r="A117" t="s">
         <v>112</v>
       </c>
-      <c r="B117" t="s">
-        <v>30</v>
-      </c>
-      <c r="C117" s="2" t="s">
+      <c r="B117" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B118" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C118" s="2" t="s">
+      <c r="B118" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C118" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2913,18 +2915,18 @@
       <c r="A119" t="s">
         <v>115</v>
       </c>
-      <c r="B119" t="s">
-        <v>30</v>
-      </c>
-      <c r="C119" s="2" t="s">
+      <c r="B119" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C120" s="2" t="s">
+      <c r="B120" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2932,18 +2934,18 @@
       <c r="A121" t="s">
         <v>118</v>
       </c>
-      <c r="B121" t="s">
-        <v>30</v>
-      </c>
-      <c r="C121" s="2" t="s">
+      <c r="B121" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B122" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C122" s="2" t="s">
+      <c r="B122" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C122" s="1" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2951,18 +2953,18 @@
       <c r="A123" t="s">
         <v>121</v>
       </c>
-      <c r="B123" t="s">
-        <v>30</v>
-      </c>
-      <c r="C123" s="2" t="s">
+      <c r="B123" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B124" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C124" s="2" t="s">
+      <c r="B124" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2970,48 +2972,48 @@
       <c r="A125" t="s">
         <v>124</v>
       </c>
-      <c r="B125" t="s">
-        <v>30</v>
-      </c>
-      <c r="C125" s="2" t="s">
+      <c r="B125" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B126" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>349</v>
+      <c r="B126" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-      <c r="B127" t="s">
-        <v>30</v>
-      </c>
-      <c r="C127" s="2" t="s">
+      <c r="B127" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B128" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C128" s="2" t="s">
+      <c r="B128" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
-      <c r="B129" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C129" s="2" t="s">
+      <c r="B129" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>130</v>
       </c>
     </row>
@@ -3019,42 +3021,42 @@
       <c r="A130" t="s">
         <v>131</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C130" s="2" t="s">
+      <c r="C130" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
-        <v>30</v>
-      </c>
-      <c r="C131" s="2" t="s">
+      <c r="B131" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B132" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C132" s="2" t="s">
+      <c r="B132" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B133" t="s">
+      <c r="B133" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B134" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C134" s="2" t="s">
+      <c r="B134" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3062,42 +3064,42 @@
       <c r="A135" t="s">
         <v>134</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>30</v>
-      </c>
-      <c r="C136" s="2" t="s">
+      <c r="B136" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B137" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C137" s="2" t="s">
+      <c r="B137" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B138" t="s">
+      <c r="B138" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C138" s="2" t="s">
+      <c r="C138" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B139" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C139" s="2" t="s">
+      <c r="B139" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C139" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3105,42 +3107,42 @@
       <c r="A140" t="s">
         <v>136</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
-        <v>30</v>
-      </c>
-      <c r="C141" s="2" t="s">
+      <c r="B141" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C141" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B142" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C142" s="2" t="s">
+      <c r="B142" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C142" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
+      <c r="B143" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C143" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B144" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C144" s="2" t="s">
+      <c r="B144" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C144" s="1" t="s">
         <v>111</v>
       </c>
     </row>
@@ -3148,18 +3150,18 @@
       <c r="A145" t="s">
         <v>138</v>
       </c>
-      <c r="B145" t="s">
-        <v>30</v>
-      </c>
-      <c r="C145" s="2" t="s">
+      <c r="B145" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B146" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C146" s="2" t="s">
+      <c r="B146" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C146" s="1" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3167,48 +3169,48 @@
       <c r="A147" t="s">
         <v>141</v>
       </c>
-      <c r="B147" t="s">
-        <v>30</v>
-      </c>
-      <c r="C147" s="2" t="s">
+      <c r="B147" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C147" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B148" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>350</v>
+      <c r="B148" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>143</v>
       </c>
-      <c r="B149" t="s">
-        <v>30</v>
-      </c>
-      <c r="C149" s="2" t="s">
+      <c r="B149" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C149" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B150" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C150" s="2" t="s">
+      <c r="B150" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C150" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>146</v>
       </c>
-      <c r="B151" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C151" s="2" t="s">
+      <c r="B151" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C151" s="1" t="s">
         <v>147</v>
       </c>
     </row>
@@ -3216,34 +3218,34 @@
       <c r="A152" t="s">
         <v>148</v>
       </c>
-      <c r="B152" t="s">
-        <v>30</v>
-      </c>
-      <c r="C152" s="2" t="s">
+      <c r="B152" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C152" s="1" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B153" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C153" s="2" t="s">
+      <c r="B153" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C153" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B154" t="s">
+      <c r="B154" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C154" s="2" t="s">
+      <c r="C154" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B155" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C155" s="2" t="s">
+      <c r="B155" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3251,18 +3253,18 @@
       <c r="A156" t="s">
         <v>151</v>
       </c>
-      <c r="B156" t="s">
-        <v>30</v>
-      </c>
-      <c r="C156" s="2" t="s">
+      <c r="B156" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C156" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B157" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C157" s="2" t="s">
+      <c r="B157" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C157" s="1" t="s">
         <v>153</v>
       </c>
     </row>
@@ -3270,18 +3272,18 @@
       <c r="A158" t="s">
         <v>154</v>
       </c>
-      <c r="B158" t="s">
-        <v>30</v>
-      </c>
-      <c r="C158" s="2" t="s">
+      <c r="B158" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B159" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C159" s="2" t="s">
+      <c r="B159" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C159" s="1" t="s">
         <v>156</v>
       </c>
     </row>
@@ -3289,26 +3291,26 @@
       <c r="A160" t="s">
         <v>157</v>
       </c>
-      <c r="B160" t="s">
-        <v>30</v>
-      </c>
-      <c r="C160" s="2" t="s">
+      <c r="B160" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C160" s="1" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B161" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>351</v>
+      <c r="B161" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
+      <c r="B162" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="1" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3316,34 +3318,34 @@
       <c r="A163" t="s">
         <v>160</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C163" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B164" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C164" s="2" t="s">
+      <c r="B164" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C164" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>30</v>
-      </c>
-      <c r="C165" s="2" t="s">
+      <c r="B165" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C165" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B166" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C166" s="2" t="s">
+      <c r="B166" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C166" s="1" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3351,15 +3353,15 @@
       <c r="B167" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C167" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B168" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C168" s="2" t="s">
+      <c r="B168" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C168" s="1" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3367,15 +3369,15 @@
       <c r="B169" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C169" s="1" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B170" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C170" s="2" t="s">
+      <c r="B170" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C170" s="1" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3383,82 +3385,82 @@
       <c r="B171" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
+      <c r="B172" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C172" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B173" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C173" s="2" t="s">
+    <row r="173" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B173" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C173" s="1" t="s">
         <v>172</v>
       </c>
       <c r="D173" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B174" t="s">
-        <v>173</v>
-      </c>
-      <c r="C174" s="2" t="s">
+      <c r="B174" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C174" s="1" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C175" s="2" t="s">
+      <c r="B175" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C175" s="1" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B176" t="s">
-        <v>173</v>
-      </c>
-      <c r="C176" s="2" t="s">
+      <c r="B176" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C176" s="1" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B177" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C177" s="2" t="s">
+      <c r="B177" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C177" s="1" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B178" t="s">
+      <c r="B178" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="C178" s="1" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B179" t="s">
-        <v>173</v>
-      </c>
-      <c r="C179" s="2" t="s">
+      <c r="B179" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C179" s="1" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B180" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C180" s="2" t="s">
+      <c r="B180" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C180" s="1" t="s">
         <v>180</v>
       </c>
     </row>
@@ -3466,10 +3468,10 @@
       <c r="A181" t="s">
         <v>181</v>
       </c>
-      <c r="B181" t="s">
-        <v>173</v>
-      </c>
-      <c r="C181" s="2" t="s">
+      <c r="B181" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C181" s="1" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3477,10 +3479,10 @@
       <c r="A182" t="s">
         <v>183</v>
       </c>
-      <c r="B182" t="s">
-        <v>173</v>
-      </c>
-      <c r="C182" s="2" t="s">
+      <c r="B182" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C182" s="1" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3488,10 +3490,10 @@
       <c r="A183" t="s">
         <v>184</v>
       </c>
-      <c r="B183" t="s">
-        <v>173</v>
-      </c>
-      <c r="C183" s="2" t="s">
+      <c r="B183" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C183" s="1" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3499,26 +3501,26 @@
       <c r="A184" t="s">
         <v>185</v>
       </c>
-      <c r="B184" t="s">
-        <v>30</v>
-      </c>
-      <c r="C184" s="2" t="s">
+      <c r="B184" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C184" s="1" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B185" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C185" s="2" t="s">
+      <c r="B185" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C185" s="1" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B186" t="s">
-        <v>173</v>
-      </c>
-      <c r="C186" s="2" t="s">
+      <c r="B186" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C186" s="1" t="s">
         <v>182</v>
       </c>
     </row>
@@ -3526,1157 +3528,1158 @@
       <c r="A187" t="s">
         <v>188</v>
       </c>
-      <c r="B187" t="s">
-        <v>173</v>
-      </c>
-      <c r="C187" s="2" t="s">
+      <c r="B187" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C187" s="1" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B188" t="s">
-        <v>30</v>
-      </c>
-      <c r="C188" s="2" t="s">
+      <c r="B188" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C188" s="1" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B189" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C189" s="2" t="s">
+      <c r="B189" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C189" s="1" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B190" t="s">
-        <v>30</v>
-      </c>
-      <c r="C190" s="2" t="s">
+      <c r="B190" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C190" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B191" t="s">
-        <v>173</v>
-      </c>
-      <c r="C191" s="2" t="s">
+      <c r="B191" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B192" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B193" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B194" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C194" s="1" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B192" t="s">
-        <v>73</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
-        <v>173</v>
-      </c>
-      <c r="C193" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B194" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C194" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>194</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C195" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="B195" t="s">
-        <v>173</v>
-      </c>
-      <c r="C195" s="2" t="s">
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B196" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B197" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B198" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C198" s="1" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B196" t="s">
-        <v>73</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>173</v>
-      </c>
-      <c r="C197" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B198" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>197</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C199" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="B199" t="s">
-        <v>173</v>
-      </c>
-      <c r="C199" s="2" t="s">
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B200" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C200" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B200" t="s">
-        <v>30</v>
-      </c>
-      <c r="C200" s="2" t="s">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B201" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C201" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B201" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C201" s="2" t="s">
+    <row r="202" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B202" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C202" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="202" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B202" t="s">
-        <v>173</v>
-      </c>
-      <c r="C202" s="2" t="s">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B203" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C203" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B203" t="s">
-        <v>73</v>
-      </c>
-      <c r="C203" s="2" t="s">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B204" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C204" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B204" t="s">
-        <v>30</v>
-      </c>
-      <c r="C204" s="2" t="s">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B205" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C205" s="1" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B205" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>205</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C206" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="B206" t="s">
-        <v>73</v>
-      </c>
-      <c r="C206" s="2" t="s">
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B207" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C207" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B207" t="s">
-        <v>30</v>
-      </c>
-      <c r="C207" s="2" t="s">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B208" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C208" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B208" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C208" s="2" t="s">
+    <row r="209" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B209" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C209" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="209" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
-        <v>173</v>
-      </c>
-      <c r="C209" s="2" t="s">
+    <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B210" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C210" s="1" t="s">
         <v>210</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B210" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>211</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C211" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B211" t="s">
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B212" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B213" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B214" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C211" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B212" t="s">
-        <v>30</v>
-      </c>
-      <c r="C212" s="2" t="s">
+      <c r="C214" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B215" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C215" s="1" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B213" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C213" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
-        <v>73</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B215" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C215" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>215</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B216" t="s">
-        <v>30</v>
-      </c>
-      <c r="C216" s="2" t="s">
+    </row>
+    <row r="217" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B217" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C217" s="1" t="s">
         <v>217</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B217" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C217" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>218</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C218" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B218" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C218" s="2" t="s">
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B219" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C219" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B219" t="s">
-        <v>30</v>
-      </c>
-      <c r="C219" s="2" t="s">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B220" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C220" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B220" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
     <row r="221" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B221" t="s">
-        <v>173</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>223</v>
+      <c r="B221" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
+        <v>222</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B223" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C223" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="B222" t="s">
-        <v>30</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B223" t="s">
-        <v>173</v>
-      </c>
-      <c r="C223" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>227</v>
-      </c>
-      <c r="B224" t="s">
-        <v>30</v>
-      </c>
-      <c r="C224" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C224" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B225" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C225" s="2" t="s">
+      <c r="B225" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C225" s="1" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
+        <v>226</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B227" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C227" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B226" t="s">
-        <v>30</v>
-      </c>
-      <c r="C226" s="2" t="s">
+    </row>
+    <row r="228" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B228" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B229" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C229" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B227" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C227" s="2" t="s">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B230" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C230" s="1" t="s">
         <v>230</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B228" t="s">
-        <v>173</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B229" t="s">
-        <v>30</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B230" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C230" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>234</v>
-      </c>
-      <c r="B231" t="s">
-        <v>173</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B232" t="s">
-        <v>30</v>
-      </c>
-      <c r="C232" s="2" t="s">
-        <v>232</v>
+      <c r="B232" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B233" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C233" s="2" t="s">
-        <v>233</v>
+      <c r="B233" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
+        <v>233</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B235" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B236" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C236" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B234" t="s">
-        <v>173</v>
-      </c>
-      <c r="C234" s="2" t="s">
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B237" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C237" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B235" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C235" s="2" t="s">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B238" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C238" s="1" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B236" t="s">
-        <v>173</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B237" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B238" t="s">
-        <v>30</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>239</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B240" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B241" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
         <v>242</v>
       </c>
-      <c r="B239" t="s">
-        <v>173</v>
-      </c>
-      <c r="C239" s="2" t="s">
+      <c r="B242" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C242" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B240" t="s">
-        <v>30</v>
-      </c>
-      <c r="C240" s="2" t="s">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B243" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C243" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B241" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C241" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="242" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>246</v>
-      </c>
-      <c r="B242" t="s">
-        <v>173</v>
-      </c>
-      <c r="C242" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B243" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B244" t="s">
-        <v>173</v>
-      </c>
-      <c r="C244" s="2" t="s">
+      <c r="B244" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C244" s="1" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>249</v>
-      </c>
-      <c r="B245" t="s">
-        <v>30</v>
-      </c>
-      <c r="C245" s="2" t="s">
-        <v>225</v>
+        <v>245</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B246" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C246" s="2" t="s">
-        <v>250</v>
+      <c r="B246" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>251</v>
-      </c>
-      <c r="B247" t="s">
-        <v>173</v>
-      </c>
-      <c r="C247" s="2" t="s">
-        <v>252</v>
+        <v>247</v>
+      </c>
+      <c r="B247" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B248" t="s">
-        <v>30</v>
-      </c>
-      <c r="C248" s="2" t="s">
+      <c r="B248" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C248" s="1" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
+        <v>249</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B250" s="4"/>
+      <c r="C250" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B251" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C251" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B249" t="s">
-        <v>173</v>
-      </c>
-      <c r="C249" s="2" t="s">
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B252" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C252" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C250" s="2" t="s">
+    <row r="253" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B253" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C253" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="251" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B251" s="5" t="s">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B254" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C254" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="C251" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B252" t="s">
-        <v>173</v>
-      </c>
-      <c r="C252" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B253" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C253" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B254" t="s">
-        <v>173</v>
-      </c>
-      <c r="C254" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
+        <v>257</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B256" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B257" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="B255" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C255" s="2" t="s">
+      <c r="C257" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B256" s="5" t="s">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B258" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C256" s="2" t="s">
+      <c r="C258" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B257" s="5" t="s">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B259" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C259" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C257" s="2" t="s">
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B260" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C260" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B258" s="5" t="s">
+    <row r="261" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B261" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B262" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C262" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="C258" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B259" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C259" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B260" t="s">
-        <v>173</v>
-      </c>
-      <c r="C260" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="261" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B261" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C261" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="262" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B262" t="s">
-        <v>173</v>
-      </c>
-      <c r="C262" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
+        <v>268</v>
+      </c>
+      <c r="B263" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B264" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B265" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C265" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="B263" t="s">
-        <v>30</v>
-      </c>
-      <c r="C263" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B264" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C264" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B265" t="s">
-        <v>275</v>
-      </c>
-      <c r="C265" s="2" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>277</v>
-      </c>
-      <c r="B266" t="s">
-        <v>30</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>278</v>
+        <v>273</v>
+      </c>
+      <c r="B266" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B267" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>279</v>
+      <c r="B267" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B268" t="s">
-        <v>275</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>276</v>
+      <c r="B268" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>280</v>
-      </c>
-      <c r="B269" t="s">
-        <v>30</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B270" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C270" s="2" t="s">
-        <v>282</v>
+      <c r="B270" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B271" t="s">
-        <v>275</v>
-      </c>
-      <c r="C271" s="2" t="s">
-        <v>276</v>
+      <c r="B271" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>283</v>
-      </c>
-      <c r="B272" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C272" s="2" t="s">
-        <v>284</v>
+        <v>279</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>285</v>
-      </c>
-      <c r="B273" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C273" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>287</v>
-      </c>
-      <c r="B274" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C274" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="275" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
+        <v>285</v>
+      </c>
+      <c r="B275" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B276" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B277" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B278" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B279" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C279" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B275" t="s">
-        <v>173</v>
-      </c>
-      <c r="C275" s="2" t="s">
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B280" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C280" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="276" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B276" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="C276" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="277" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B277" t="s">
-        <v>173</v>
-      </c>
-      <c r="C277" s="2" t="s">
+    <row r="281" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B281" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C281" s="1" t="s">
         <v>291</v>
-      </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B278" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C278" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B279" t="s">
-        <v>73</v>
-      </c>
-      <c r="C279" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B280" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C280" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B281" t="s">
-        <v>173</v>
-      </c>
-      <c r="C281" s="2" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="282" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
+        <v>292</v>
+      </c>
+      <c r="B282" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B283" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B284" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B285" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B286" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B287" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B288" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B289" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C289" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B282" t="s">
-        <v>173</v>
-      </c>
-      <c r="C282" s="2" t="s">
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B290" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C290" s="1" t="s">
         <v>297</v>
-      </c>
-    </row>
-    <row r="283" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B283" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C283" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B284" t="s">
-        <v>173</v>
-      </c>
-      <c r="C284" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B285" t="s">
-        <v>173</v>
-      </c>
-      <c r="C285" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B286" t="s">
-        <v>173</v>
-      </c>
-      <c r="C286" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B287" t="s">
-        <v>173</v>
-      </c>
-      <c r="C287" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B288" t="s">
-        <v>173</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B289" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C289" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B290" t="s">
-        <v>173</v>
-      </c>
-      <c r="C290" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
+        <v>298</v>
+      </c>
+      <c r="B291" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B292" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B293" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B294" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B295" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B296" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B297" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B298" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C298" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="B291" t="s">
-        <v>173</v>
-      </c>
-      <c r="C291" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="292" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B292" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C292" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B293" t="s">
-        <v>173</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="294" spans="1:3" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B294" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C294" s="4" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="295" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B295" t="s">
-        <v>173</v>
-      </c>
-      <c r="C295" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B296" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C296" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B297" t="s">
-        <v>173</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B298" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C298" s="2" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
+        <v>304</v>
+      </c>
+      <c r="B299" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B300" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B301" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B302" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B303" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B304" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C306" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="B308" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B310" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C310" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="B299" t="s">
-        <v>173</v>
-      </c>
-      <c r="C299" s="2" t="s">
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C312" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="300" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B300" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C300" s="2" t="s">
+    <row r="313" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B313" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C313" s="1" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B301" t="s">
-        <v>173</v>
-      </c>
-      <c r="C301" s="2" t="s">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B314" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C314" s="1" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B302" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C302" s="2" t="s">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B315" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C315" s="1" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B303" t="s">
-        <v>173</v>
-      </c>
-      <c r="C303" s="2" t="s">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B316" s="3" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B304" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C304" s="2" t="s">
+      <c r="C316" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="306" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="C306" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="308" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="B308" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C308" s="2" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="310" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B310" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="C310" s="2" t="s">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B317" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C317" s="1" t="s">
         <v>317</v>
-      </c>
-    </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C312" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B313" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C313" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B314" t="s">
-        <v>173</v>
-      </c>
-      <c r="C314" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B315" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="C315" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B316" t="s">
-        <v>322</v>
-      </c>
-      <c r="C316" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B317" t="s">
-        <v>1</v>
-      </c>
-      <c r="C317" s="2" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
+        <v>318</v>
+      </c>
+      <c r="B318" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C319" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C320" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C321" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C322" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C323" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C325" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="B318" t="s">
-        <v>1</v>
-      </c>
-      <c r="C318" s="2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C319" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C320" s="2" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C321" s="2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C322" s="2" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C323" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C325" s="2" t="s">
-        <v>332</v>
-      </c>
     </row>
     <row r="329" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C329" s="2" t="s">
-        <v>342</v>
+      <c r="C329" s="1" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="330" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C330" s="2" t="s">
-        <v>343</v>
+      <c r="C330" s="1" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="331" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C331" s="2" t="s">
-        <v>344</v>
+      <c r="C331" s="1" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="332" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C332" s="2" t="s">
-        <v>345</v>
+      <c r="C332" s="1" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="333" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C333" s="2" t="s">
-        <v>346</v>
+      <c r="C333" s="1" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
few more changes while recording
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Story/Resources/Story.xlsx
+++ b/Assets/Scripts/Story/Resources/Story.xlsx
@@ -93,9 +93,6 @@
     <t>Yaaay! That is so great to hear. We are going on an adventure together. It is going to be awesome! Let’s start connecting you to a spirit bear now. Amazing what technology can do nowadays.</t>
   </si>
   <si>
-    <t>Neh, it is okay. Whoever said technology would replace all paper obviously hasn't tried wiping their butt with an IPad…ha. ha. ha…. Starting connection in 3… 2… 1…</t>
-  </si>
-  <si>
     <t>*connection sounds*</t>
   </si>
   <si>
@@ -1099,6 +1096,9 @@
   </si>
   <si>
     <t>Ahhh *hoooot* home sweet home. Thank you human, for your exceptional help. You are very talented, and will achieve many great things!! I'll soon bring these science birds back to science land.</t>
+  </si>
+  <si>
+    <t>You are wrong. Whoever said technology would replace all paper obviously hasn't tried wiping their butt with an IPad…ha. ha. ha…. Starting connection in 3… 2… 1…</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1445,6 +1445,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1606,7 +1612,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1616,6 +1622,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1939,8 +1946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="C314" sqref="C314"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1961,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1985,7 +1992,7 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1994,10 +2001,10 @@
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -2005,7 +2012,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
@@ -2015,7 +2022,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2024,14 +2031,14 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2040,14 +2047,14 @@
     </row>
     <row r="13" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2056,14 +2063,14 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2072,10 +2079,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2083,7 +2090,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -2094,7 +2101,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -2104,7 +2111,7 @@
       <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2113,2573 +2120,2572 @@
     </row>
     <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="1" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>30</v>
+        <v>45</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>30</v>
+        <v>47</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>30</v>
+        <v>49</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>30</v>
+        <v>55</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C59" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>30</v>
+        <v>63</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>71</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>30</v>
+        <v>70</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C73" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C73" s="1" t="s">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C80" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C82" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>81</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>30</v>
+        <v>80</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B88" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C88" s="1" t="s">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B91" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C98" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B100" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="C102" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C104" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>100</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>105</v>
-      </c>
-      <c r="B109" s="3" t="s">
-        <v>30</v>
+        <v>104</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>107</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>111</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>114</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B119" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>117</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>120</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>123</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="B125" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>125</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C127" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B129" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="C130" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C130" s="1" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B131" s="3" t="s">
-        <v>30</v>
+      <c r="B131" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>133</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C135" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B135" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>135</v>
-      </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B136" s="3" t="s">
-        <v>30</v>
+      <c r="B136" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B138" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
+        <v>135</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C140" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B140" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C140" s="1" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B141" s="3" t="s">
-        <v>30</v>
+      <c r="B141" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
+        <v>137</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C145" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
+        <v>140</v>
+      </c>
+      <c r="B147" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C147" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B147" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>142</v>
+      </c>
+      <c r="B149" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C149" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B149" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B150" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C150" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="B151" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C151" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>148</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>30</v>
+        <v>147</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B153" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B155" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C156" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B157" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>153</v>
+      </c>
+      <c r="B158" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B159" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
+        <v>156</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C160" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="B160" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B161" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B162" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
+        <v>159</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C163" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C163" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B164" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C164" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B165" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C165" s="1" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B165" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B166" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B167" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C167" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C167" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B168" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B169" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B170" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B171" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B172" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B173" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D173" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B174" s="4" t="s">
+      <c r="B174" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C174" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="C174" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B175" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C175" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B176" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C176" s="1" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B176" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C176" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B177" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B178" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C178" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B179" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C179" s="1" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B179" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C179" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B180" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
+        <v>180</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C181" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C181" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>183</v>
-      </c>
-      <c r="B182" s="4" t="s">
-        <v>173</v>
+        <v>182</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>184</v>
-      </c>
-      <c r="B183" s="4" t="s">
-        <v>173</v>
+        <v>183</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
+        <v>184</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C184" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="B184" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C184" s="1" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B185" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B186" s="4" t="s">
-        <v>173</v>
+      <c r="B186" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
+        <v>187</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C187" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B187" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C187" s="1" t="s">
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B188" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C188" s="1" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B188" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C188" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B189" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C189" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B190" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C190" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B190" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C190" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
     <row r="191" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B191" s="4" t="s">
-        <v>173</v>
+      <c r="B191" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B192" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C192" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B193" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C193" s="1" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B193" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C193" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B194" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
+        <v>193</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C195" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="B195" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C195" s="1" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B196" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C196" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B197" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C197" s="1" t="s">
         <v>178</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B197" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B198" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
+        <v>196</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C199" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B199" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C199" s="1" t="s">
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B200" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C200" s="1" t="s">
         <v>198</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B200" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C200" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B201" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C201" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B202" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C202" s="1" t="s">
         <v>200</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B202" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B203" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C203" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B204" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C204" s="1" t="s">
         <v>202</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B204" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B205" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
+        <v>204</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C206" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B206" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C206" s="1" t="s">
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B207" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C207" s="1" t="s">
         <v>206</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B207" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C207" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B208" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C208" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B209" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C209" s="1" t="s">
         <v>208</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B209" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B210" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
+        <v>210</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C211" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B211" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C211" s="1" t="s">
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B212" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C212" s="1" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B212" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B213" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B214" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B215" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
+        <v>214</v>
+      </c>
+      <c r="B216" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C216" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B216" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B217" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>217</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C218" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B218" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C218" s="1" t="s">
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B219" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C219" s="1" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B219" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C219" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B220" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B221" s="4" t="s">
-        <v>173</v>
+      <c r="B221" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
+        <v>221</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C222" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B222" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C222" s="1" t="s">
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B223" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C223" s="1" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B223" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>225</v>
-      </c>
-      <c r="B224" s="3" t="s">
-        <v>30</v>
+        <v>224</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B225" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
+        <v>225</v>
+      </c>
+      <c r="B226" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C226" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="B226" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B227" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C227" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B228" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B229" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C229" s="1" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B228" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B229" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B230" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
+        <v>230</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C231" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B231" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C231" s="1" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B232" s="3" t="s">
-        <v>30</v>
+      <c r="B232" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B233" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
+        <v>232</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C234" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B234" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B235" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C235" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B236" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C236" s="1" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B236" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B237" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C237" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B238" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C238" s="1" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B238" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
+        <v>238</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B240" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C240" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="B239" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C239" s="1" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B240" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C240" s="1" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B241" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
+        <v>241</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C242" s="1" t="s">
         <v>242</v>
-      </c>
-      <c r="B242" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C242" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B243" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C243" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B244" s="4" t="s">
-        <v>173</v>
+      <c r="B244" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>245</v>
-      </c>
-      <c r="B245" s="3" t="s">
-        <v>30</v>
+        <v>244</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B246" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
+        <v>246</v>
+      </c>
+      <c r="B247" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C247" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B247" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C247" s="1" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B248" s="3" t="s">
-        <v>30</v>
+      <c r="B248" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
+        <v>248</v>
+      </c>
+      <c r="B249" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C249" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B249" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C249" s="1" t="s">
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C250" s="1" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B250" s="4"/>
-      <c r="C250" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B251" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C251" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C251" s="1" t="s">
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B252" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C252" s="1" t="s">
         <v>253</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B252" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B253" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C253" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B254" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C254" s="1" t="s">
         <v>255</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B254" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
+        <v>256</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C255" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="B255" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B256" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C256" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B257" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C257" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B258" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C258" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B259" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C259" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B260" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C260" s="1" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B260" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C260" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="261" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B261" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B262" s="4" t="s">
-        <v>173</v>
+      <c r="B262" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
+        <v>267</v>
+      </c>
+      <c r="B263" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C263" s="1" t="s">
         <v>268</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B264" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B265" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C265" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="C265" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
+        <v>272</v>
+      </c>
+      <c r="B266" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C266" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C266" s="1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B267" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B268" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C268" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="C268" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
+        <v>275</v>
+      </c>
+      <c r="B269" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C269" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="B269" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C269" s="1" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B270" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B271" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C271" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="C271" s="1" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
+        <v>278</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C272" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
+        <v>280</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C273" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="B273" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C273" s="1" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
+        <v>282</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C274" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="B274" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="C274" s="1" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="275" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
+        <v>284</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C275" s="1" t="s">
         <v>285</v>
-      </c>
-      <c r="B275" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C275" s="1" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B276" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B277" s="4" t="s">
-        <v>173</v>
+      <c r="B277" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B278" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B279" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B280" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C280" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B281" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C281" s="1" t="s">
         <v>290</v>
-      </c>
-    </row>
-    <row r="281" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B281" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C281" s="1" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="282" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
+        <v>291</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C282" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="B282" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C282" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="283" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B283" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B284" s="4" t="s">
-        <v>173</v>
+      <c r="B284" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B285" s="4" t="s">
-        <v>173</v>
+      <c r="B285" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C285" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B286" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B287" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B288" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C288" s="1" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B286" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C286" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B287" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C287" s="1" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B288" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B289" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C289" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B290" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C290" s="1" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B290" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="291" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
+        <v>297</v>
+      </c>
+      <c r="B291" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C291" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="B291" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C291" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="B292" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B293" s="4" t="s">
-        <v>173</v>
+      <c r="B293" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B294" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C294" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B295" s="4" t="s">
-        <v>173</v>
+      <c r="B295" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B296" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C296" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B297" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C297" s="1" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="297" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B297" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C297" s="1" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B298" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>304</v>
-      </c>
-      <c r="B299" s="4" t="s">
-        <v>173</v>
+        <v>303</v>
+      </c>
+      <c r="B299" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="300" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B300" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C300" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B301" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C301" s="1" t="s">
         <v>305</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B301" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C301" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B302" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C302" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B303" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C303" s="1" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B303" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C303" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B304" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C306" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="B308" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B310" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C312" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B313" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C313" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B314" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C314" s="1" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B314" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C314" s="1" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B315" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B316" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C316" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C316" s="1" t="s">
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B317" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C317" s="1" t="s">
         <v>316</v>
-      </c>
-    </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B317" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C317" s="1" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
+        <v>317</v>
+      </c>
+      <c r="B318" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C318" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="B318" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C318" s="1" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C319" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C320" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="321" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C321" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="322" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C322" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="323" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C323" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="325" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C325" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="329" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C329" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="330" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C330" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="331" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C331" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="332" spans="3:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C332" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="333" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C333" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>